<commit_message>
Corrected a version number
</commit_message>
<xml_diff>
--- a/FMAC_FW_Versions.xlsx
+++ b/FMAC_FW_Versions.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Projects\Murata\In progress\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MEAASC01\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B31C6E-CDAA-41EC-99E4-5EBC0BC86FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7CD3ECA7-551E-4D03-8AE3-894C4CB75349}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28860" windowHeight="11220"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,12 +35,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Romit Chatterjee</author>
   </authors>
   <commentList>
-    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{D49169AA-9EA8-4F3B-AF7D-10CB10A9DE38}">
+    <comment ref="G2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -494,7 +493,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1262,7 +1261,6 @@
         <sz val="11"/>
         <color auto="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -1292,7 +1290,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Table Style 1" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Table Style 1" pivot="0" count="1" xr9:uid="{5135CE5A-4A8D-401E-9344-7F6A05CA89C6}">
+    <tableStyle name="Table Style 1" pivot="0" count="1">
       <tableStyleElement type="headerRow" dxfId="24"/>
     </tableStyle>
   </tableStyles>
@@ -1314,32 +1312,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4C589FC3-6793-42D5-8660-E56E7EBF6C94}" name="Table1" displayName="Table1" ref="A1:T16" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
-  <autoFilter ref="A1:T16" xr:uid="{4C589FC3-6793-42D5-8660-E56E7EBF6C94}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:T16" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+  <autoFilter ref="A1:T16"/>
+  <sortState ref="A2:T16">
     <sortCondition ref="A1:A16"/>
   </sortState>
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{B19F32F1-C65E-49D9-B7DA-9B614B90FB40}" name="FW name" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{C6249642-B74D-4BB3-9A84-5C1AB6C070FC}" name="Module" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{F4926B77-3FA2-426F-88A0-82C5C5647DA4}" name="Chipset" dataDxfId="17"/>
-    <tableColumn id="20" xr3:uid="{14825DA6-9289-4526-B7A1-CB8B223781F2}" name="Jaculus_x000a_(v6.1.97-2024_1115)" dataDxfId="16" dataCellStyle="Hyperlink"/>
-    <tableColumn id="19" xr3:uid="{EBA9E9A0-600F-4855-A873-A1F7DCC076AA}" name="Indrik_x000a_(v5.15.58-2024_0514)" dataDxfId="15" dataCellStyle="Hyperlink"/>
-    <tableColumn id="18" xr3:uid="{792F1E4D-0DD5-4ED0-BF4B-4C5B8D26B683}" name="Hedorah_x000a_(v5.15.58-2023_1128)" dataDxfId="14" dataCellStyle="Hyperlink"/>
-    <tableColumn id="17" xr3:uid="{B896F0AC-A937-4008-B225-2CBB28E5ED54}" name="Godzilla 3_x000a_(v5.15.58-2023_0901)" dataDxfId="13" dataCellStyle="Hyperlink"/>
-    <tableColumn id="16" xr3:uid="{F68B6DAF-D6B3-4F7F-ABB1-A1BBAA32BAA2}" name="Godzilla 2_x000a_(v5.15.58-2023_0801)" dataDxfId="12" dataCellStyle="Hyperlink"/>
-    <tableColumn id="15" xr3:uid="{957C99B4-F985-4422-B227-6CF56539EC5C}" name="Godzilla_x000a_(v5.15.58-2023_0523)" dataDxfId="11" dataCellStyle="Hyperlink"/>
-    <tableColumn id="14" xr3:uid="{C492B750-5699-4243-B781-5D531AB1B3E1}" name="Fafnir 2_x000a_(v5.15.58-2023_0222)" dataDxfId="10" dataCellStyle="Hyperlink"/>
-    <tableColumn id="13" xr3:uid="{A912F632-97A7-4216-A801-5ABD4789ED16}" name="Fafnir_x000a_(v5.15.58-20221223)" dataDxfId="9" dataCellStyle="Hyperlink"/>
-    <tableColumn id="12" xr3:uid="{E02216FA-3406-4E36-A5E5-C7F809862F31}" name="Ebirah_x000a_(v5.10.9-2022_0909)" dataDxfId="8" dataCellStyle="Hyperlink"/>
-    <tableColumn id="11" xr3:uid="{8B02E047-9204-4795-83A2-C0B6C6708E96}" name="Drogon_x000a_(v5.10.9-2022_0511)" dataDxfId="7" dataCellStyle="Hyperlink"/>
-    <tableColumn id="10" xr3:uid="{C048E657-6E74-41A4-8682-48A447592B05}" name="Cynder_x000a_(v5.10.9-2021_1020)" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{DB45AA24-B366-414D-B42A-1DDD99C5CC17}" name="Baragon_x000a_(v5.4.18-2021_0527)" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{C2390AC6-296F-4744-8FF4-56D29D512B05}" name="Spiga_x000a_(v5.4.18-2020_0925)" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{806DA1E0-DFD2-4F88-A0EE-1C7D4BB55884}" name="Zigra_x000a_(v5.4.18-2020_0625)" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{01679B73-F7D3-4C39-850E-D91E778C7214}" name="Kong_x000a_(v4.14.77-2020_0115)" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{C0694E67-27EB-48A9-891E-2B07AE60CC9F}" name="Manda_x000a_(v4.14.52-2018_0928)" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{C778F452-7E64-467E-96D9-53B85D1DC4EA}" name="Mothra_x000a_(v4.14.34-2018_0716)" dataDxfId="0"/>
+    <tableColumn id="1" name="FW name" dataDxfId="19"/>
+    <tableColumn id="2" name="Module" dataDxfId="18"/>
+    <tableColumn id="3" name="Chipset" dataDxfId="17"/>
+    <tableColumn id="20" name="Jaculus_x000a_(v6.1.97-2024_1115)" dataDxfId="16" dataCellStyle="Hyperlink"/>
+    <tableColumn id="19" name="Indrik_x000a_(v5.15.58-2024_0514)" dataDxfId="15" dataCellStyle="Hyperlink"/>
+    <tableColumn id="18" name="Hedorah_x000a_(v5.15.58-2023_1128)" dataDxfId="14" dataCellStyle="Hyperlink"/>
+    <tableColumn id="17" name="Godzilla 3_x000a_(v5.15.58-2023_0901)" dataDxfId="13" dataCellStyle="Hyperlink"/>
+    <tableColumn id="16" name="Godzilla 2_x000a_(v5.15.58-2023_0801)" dataDxfId="12" dataCellStyle="Hyperlink"/>
+    <tableColumn id="15" name="Godzilla_x000a_(v5.15.58-2023_0523)" dataDxfId="11" dataCellStyle="Hyperlink"/>
+    <tableColumn id="14" name="Fafnir 2_x000a_(v5.15.58-2023_0222)" dataDxfId="10" dataCellStyle="Hyperlink"/>
+    <tableColumn id="13" name="Fafnir_x000a_(v5.15.58-20221223)" dataDxfId="9" dataCellStyle="Hyperlink"/>
+    <tableColumn id="12" name="Ebirah_x000a_(v5.10.9-2022_0909)" dataDxfId="8" dataCellStyle="Hyperlink"/>
+    <tableColumn id="11" name="Drogon_x000a_(v5.10.9-2022_0511)" dataDxfId="7" dataCellStyle="Hyperlink"/>
+    <tableColumn id="10" name="Cynder_x000a_(v5.10.9-2021_1020)" dataDxfId="6"/>
+    <tableColumn id="9" name="Baragon_x000a_(v5.4.18-2021_0527)" dataDxfId="5"/>
+    <tableColumn id="8" name="Spiga_x000a_(v5.4.18-2020_0925)" dataDxfId="4"/>
+    <tableColumn id="7" name="Zigra_x000a_(v5.4.18-2020_0625)" dataDxfId="3"/>
+    <tableColumn id="6" name="Kong_x000a_(v4.14.77-2020_0115)" dataDxfId="2"/>
+    <tableColumn id="5" name="Manda_x000a_(v4.14.52-2018_0928)" dataDxfId="1"/>
+    <tableColumn id="4" name="Mothra_x000a_(v4.14.34-2018_0716)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1641,14 +1639,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B65CE068-70FE-4796-97AE-3A6AE349CBF3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:MQ23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2636,7 +2634,7 @@
         <v>73</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>64</v>
@@ -2828,170 +2826,170 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1" xr:uid="{0E442CC6-DFD9-41E8-8749-32714D2A7CB2}"/>
-    <hyperlink ref="P4" r:id="rId2" xr:uid="{0E357E19-3C23-4021-A9CE-91014E7E0D27}"/>
-    <hyperlink ref="P6" r:id="rId3" xr:uid="{715EE362-CDD2-4784-AEF0-FB0EF6A4E14F}"/>
-    <hyperlink ref="P7" r:id="rId4" xr:uid="{7526C40F-9F52-49F0-8D1F-8B694D4A5B0F}"/>
-    <hyperlink ref="Q2" r:id="rId5" xr:uid="{66D17117-5D8D-449F-BEB4-8261EEB21056}"/>
-    <hyperlink ref="Q4" r:id="rId6" xr:uid="{C5FFB072-89AA-45F8-A9B4-3757C53BFA82}"/>
-    <hyperlink ref="Q6" r:id="rId7" xr:uid="{286DB28E-EDE1-464E-B57E-36FA42559A3D}"/>
-    <hyperlink ref="Q7" r:id="rId8" xr:uid="{951B4395-D66D-4F52-B10B-E90E37D0074D}"/>
-    <hyperlink ref="Q12" r:id="rId9" xr:uid="{5B2A53B3-71A3-46F5-89DE-85BBFCFBD918}"/>
-    <hyperlink ref="Q13" r:id="rId10" xr:uid="{DE1DA4E4-A066-435F-8886-71BF45A256C5}"/>
-    <hyperlink ref="R2" r:id="rId11" xr:uid="{BCAE2F22-5777-49F7-8B27-A89AF204E7B9}"/>
-    <hyperlink ref="R4" r:id="rId12" xr:uid="{0DC4DABD-879E-4BD7-B1B9-87B03C077AA1}"/>
-    <hyperlink ref="R6" r:id="rId13" xr:uid="{5C22A346-3A01-4E06-A661-AC73096EE6B1}"/>
-    <hyperlink ref="R7" r:id="rId14" xr:uid="{4DC54413-DA99-4E6D-9662-16BEFAFFDB50}"/>
-    <hyperlink ref="S2" r:id="rId15" xr:uid="{B967F5FD-6503-4BAB-979A-F4118D3CB4E9}"/>
-    <hyperlink ref="S4" r:id="rId16" xr:uid="{8722875F-4A0F-4106-A7C4-B9E0C633C5A5}"/>
-    <hyperlink ref="S6" r:id="rId17" xr:uid="{EDCA83D7-F0A8-4E7A-BEBC-D76346175224}"/>
-    <hyperlink ref="T2" r:id="rId18" xr:uid="{D6B91A77-7407-4A7F-A2B1-4D13324E6A2B}"/>
-    <hyperlink ref="T4" r:id="rId19" xr:uid="{747C6FCC-BC34-4BAA-B1CD-495256D5DAB7}"/>
-    <hyperlink ref="T6" r:id="rId20" xr:uid="{4A93EFA5-F2AF-43B5-B12E-618AD9AF6325}"/>
-    <hyperlink ref="D2" r:id="rId21" xr:uid="{AE98C763-A813-4BD0-83C4-95EE4461B8C4}"/>
-    <hyperlink ref="D3" r:id="rId22" xr:uid="{5C37D9BB-0043-4F0D-954B-D6D1CFBE9711}"/>
-    <hyperlink ref="D5" r:id="rId23" xr:uid="{78E21A64-3589-4796-AAB9-2AB1EA1488FE}"/>
-    <hyperlink ref="D6" r:id="rId24" xr:uid="{31B5FA95-9259-42F0-9E94-8D07F90AB3BC}"/>
-    <hyperlink ref="D7" r:id="rId25" xr:uid="{864B540F-12A3-43AD-BF8C-733051D5D7EF}"/>
-    <hyperlink ref="D9" r:id="rId26" xr:uid="{FD4B2C3F-A39C-4417-9E2D-BF32EA1C86D5}"/>
-    <hyperlink ref="D12" r:id="rId27" xr:uid="{EF4A8E17-6EDD-45CD-B9B8-3E7E9C5B298C}"/>
-    <hyperlink ref="D13" r:id="rId28" xr:uid="{DAF46C09-82CB-42A8-8A1A-7743B878152B}"/>
-    <hyperlink ref="D15" r:id="rId29" xr:uid="{D336F610-A412-4A62-B0FB-89974BF466F0}"/>
-    <hyperlink ref="D16" r:id="rId30" xr:uid="{3A69C799-9D30-42E3-B00D-23B888F6424D}"/>
-    <hyperlink ref="E2" r:id="rId31" xr:uid="{64C362C9-DCAC-436B-964A-6C2291470A36}"/>
-    <hyperlink ref="E3" r:id="rId32" xr:uid="{7EE25230-DCBA-48A6-9CD8-2804EB223B00}"/>
-    <hyperlink ref="D14" r:id="rId33" xr:uid="{60C39CAA-2603-45AE-84F5-2E4E126A8373}"/>
-    <hyperlink ref="E5" r:id="rId34" xr:uid="{739A2C91-001D-447D-96BE-4255D9D6FF9F}"/>
-    <hyperlink ref="E7" r:id="rId35" xr:uid="{1D5A34CE-088B-4D3A-A7B2-60F9990F1E1B}"/>
-    <hyperlink ref="E9" r:id="rId36" xr:uid="{B117B4E3-E8BD-4931-B6CC-1E40C243EE30}"/>
-    <hyperlink ref="E12" r:id="rId37" xr:uid="{058CE23E-34B1-4C50-9404-CF5D6B905419}"/>
-    <hyperlink ref="E13" r:id="rId38" xr:uid="{12820D09-3932-4B67-94F3-C7681EEE05B4}"/>
-    <hyperlink ref="E15" r:id="rId39" xr:uid="{3165CDA0-90B8-44D8-84B1-F630EB236EA3}"/>
-    <hyperlink ref="E16" r:id="rId40" xr:uid="{C1B87295-DFA0-49B5-9570-88B8EDCA89D8}"/>
-    <hyperlink ref="F2" r:id="rId41" xr:uid="{7DC29A8F-9D25-4621-A7F0-8628DFE98001}"/>
-    <hyperlink ref="F5" r:id="rId42" xr:uid="{CE1B6265-E48B-49BF-B53B-B6DF31D1142B}"/>
-    <hyperlink ref="F7" r:id="rId43" xr:uid="{84C975FA-D640-44E0-AAF8-B04E0655F12A}"/>
-    <hyperlink ref="F9" r:id="rId44" xr:uid="{706289F6-4C74-42A7-ADBA-EC5CDC7D5808}"/>
-    <hyperlink ref="F12" r:id="rId45" xr:uid="{36C959ED-5EED-4FEF-B691-5A7BAADC2F8B}"/>
-    <hyperlink ref="F13" r:id="rId46" xr:uid="{17C3607C-B41E-484C-90B3-2CC4E88153B3}"/>
-    <hyperlink ref="F15" r:id="rId47" xr:uid="{73D70DE6-4F06-4FB5-8B7E-9CF470169C57}"/>
-    <hyperlink ref="F16" r:id="rId48" xr:uid="{76891689-CD5D-4BEC-8C05-A243C7A15796}"/>
-    <hyperlink ref="G2" r:id="rId49" xr:uid="{66A6E3D2-AD2A-4977-A535-241032F02CDD}"/>
-    <hyperlink ref="G5" r:id="rId50" xr:uid="{6FEF0B90-FB0B-41F6-9E39-E598AD9D5A5A}"/>
-    <hyperlink ref="G6" r:id="rId51" xr:uid="{F8E6839D-96F9-4A6C-9202-69C026035ABA}"/>
-    <hyperlink ref="G7" r:id="rId52" xr:uid="{410FF926-9001-49BC-8B82-C92506CCA80D}"/>
-    <hyperlink ref="G9" r:id="rId53" xr:uid="{AA353474-FB42-4F90-8D8A-2EB8AE4F8419}"/>
-    <hyperlink ref="G12" r:id="rId54" xr:uid="{7539D21D-9CFD-4916-A551-E28DA2EFF8C1}"/>
-    <hyperlink ref="G13" r:id="rId55" xr:uid="{F72C7865-2DCA-4195-A3D7-984315F95F32}"/>
-    <hyperlink ref="G15" r:id="rId56" xr:uid="{3F761014-AF48-47DB-B157-341AF9F164D0}"/>
-    <hyperlink ref="G16" r:id="rId57" xr:uid="{B6EF28CE-C6C0-485A-85C3-31260ADC7E20}"/>
-    <hyperlink ref="H2" r:id="rId58" xr:uid="{2E04928D-91CC-43FA-9362-EE7CDD5A5E83}"/>
-    <hyperlink ref="H5" r:id="rId59" xr:uid="{34D87CA5-F4FC-423B-9F06-DA3DA4A35B0B}"/>
-    <hyperlink ref="H7" r:id="rId60" xr:uid="{94EE622C-A4E7-4630-918C-2E17B88CC4EF}"/>
-    <hyperlink ref="H9" r:id="rId61" xr:uid="{8E8385B3-5B8C-46AF-AD96-41BAA27D5521}"/>
-    <hyperlink ref="H12" r:id="rId62" xr:uid="{38EA77F3-9112-4B93-82AF-0CD72FD74F84}"/>
-    <hyperlink ref="H13" r:id="rId63" xr:uid="{5A83A4F6-F89D-4698-9D2D-1669041EDB0E}"/>
-    <hyperlink ref="H15" r:id="rId64" xr:uid="{6E82DCC6-F865-4C24-95C0-DDCAB0FDBC47}"/>
-    <hyperlink ref="H16" r:id="rId65" xr:uid="{640F1131-EAB8-49F5-A718-3F1F41194628}"/>
-    <hyperlink ref="I2" r:id="rId66" xr:uid="{0B9B8085-6371-4E90-8F60-C800E3DE2A62}"/>
-    <hyperlink ref="I5" r:id="rId67" xr:uid="{978AE546-509A-4E6C-A1C3-A55869FB9EFD}"/>
-    <hyperlink ref="I7" r:id="rId68" xr:uid="{0C8B9604-662D-4BDE-A9D0-CC36BABCAA88}"/>
-    <hyperlink ref="I9" r:id="rId69" xr:uid="{159BCA08-811C-4E7B-8D2F-87FB6326D908}"/>
-    <hyperlink ref="I12" r:id="rId70" xr:uid="{3C5D5A24-8F6E-47E2-BFD5-4921DB65523A}"/>
-    <hyperlink ref="I13" r:id="rId71" xr:uid="{74974657-84E3-4ECC-B3D9-73075ECD2247}"/>
-    <hyperlink ref="I15" r:id="rId72" xr:uid="{471DDFA6-70DE-4043-A9B2-240B8A1FD9E4}"/>
-    <hyperlink ref="I16" r:id="rId73" xr:uid="{262A84BF-7E5F-404D-B2C2-3EBDBACA5E4E}"/>
-    <hyperlink ref="J2" r:id="rId74" xr:uid="{771239DD-788F-45D8-AAE0-3F645020D84D}"/>
-    <hyperlink ref="J5" r:id="rId75" xr:uid="{67F11590-B21D-43B8-A588-8F651C362C19}"/>
-    <hyperlink ref="J7" r:id="rId76" xr:uid="{A8A7D12B-AE57-420E-90AC-0E04A193A6C4}"/>
-    <hyperlink ref="J9" r:id="rId77" xr:uid="{F32562EC-DFDC-4800-9581-9428178EA4D4}"/>
-    <hyperlink ref="J12" r:id="rId78" xr:uid="{8C0294D4-C91A-4F7C-9E12-A337AEC894BC}"/>
-    <hyperlink ref="J13" r:id="rId79" xr:uid="{4AA80FB0-213C-4AC1-A3B5-261BDF59E60E}"/>
-    <hyperlink ref="J15" r:id="rId80" xr:uid="{6D80C07B-6FD6-44B0-B513-83D5C34FFA23}"/>
-    <hyperlink ref="J16" r:id="rId81" xr:uid="{9487169D-D3A5-4BF7-A567-9C09606308D1}"/>
-    <hyperlink ref="L2" r:id="rId82" xr:uid="{6A5DB995-808C-4EC4-B56E-7CA105ADDD2A}"/>
-    <hyperlink ref="L4" r:id="rId83" xr:uid="{2FA0463B-1DD4-4E9A-BD53-AF2239F97839}"/>
-    <hyperlink ref="L5" r:id="rId84" xr:uid="{503AE0C5-2973-4D16-B7BE-E3C786B4E596}"/>
-    <hyperlink ref="L6" r:id="rId85" xr:uid="{34A5463B-B734-4DEC-8BF8-EAA1A1FC3D69}"/>
-    <hyperlink ref="L7" r:id="rId86" xr:uid="{F8624665-31F5-4887-A6F4-BB93F4FD2F12}"/>
-    <hyperlink ref="L9" r:id="rId87" xr:uid="{11A9F1D7-88FF-4B7F-A134-A006A671D204}"/>
-    <hyperlink ref="L12" r:id="rId88" xr:uid="{32FD30BB-3158-4E0B-8BB6-EFAF0E275431}"/>
-    <hyperlink ref="L13" r:id="rId89" xr:uid="{C1CB9C74-8087-450F-9C55-758C6C7DDF20}"/>
-    <hyperlink ref="L15" r:id="rId90" xr:uid="{060183C9-E37F-4A47-A7E7-A4BB16F3215A}"/>
-    <hyperlink ref="L16" r:id="rId91" xr:uid="{E3520039-92DA-478F-BF2E-905D3649F2CE}"/>
-    <hyperlink ref="M2" r:id="rId92" xr:uid="{461248B5-A3DD-4B59-9E2B-0A48BDB5D77F}"/>
-    <hyperlink ref="M4" r:id="rId93" xr:uid="{557C0017-99C8-467F-9923-770A823B3728}"/>
-    <hyperlink ref="M5" r:id="rId94" xr:uid="{1B6E2B16-7BEB-436D-9879-375EAED4E9A9}"/>
-    <hyperlink ref="M6" r:id="rId95" xr:uid="{0562E965-C00E-4888-8604-8707EE7BC836}"/>
-    <hyperlink ref="M7" r:id="rId96" xr:uid="{5C1AE1E1-6092-4848-827F-8B3B71315550}"/>
-    <hyperlink ref="M9" r:id="rId97" xr:uid="{05DF5906-1FF7-4FCF-B10A-D855E1B9C96D}"/>
-    <hyperlink ref="M12" r:id="rId98" xr:uid="{BFDDDA8E-1976-411D-8CE5-CA35C32FD250}"/>
-    <hyperlink ref="M13" r:id="rId99" xr:uid="{66A99983-D75C-4DF5-9637-519B28316877}"/>
-    <hyperlink ref="N2" r:id="rId100" xr:uid="{F4ED6811-62A8-478A-B227-8811DBD8D5FC}"/>
-    <hyperlink ref="N4" r:id="rId101" xr:uid="{907945BE-9BEC-4EDE-AF53-CC64710B74D6}"/>
-    <hyperlink ref="N5" r:id="rId102" xr:uid="{CC536F13-1FC3-4691-B4C7-DB55D5BD5049}"/>
-    <hyperlink ref="N6" r:id="rId103" xr:uid="{0F1E4E60-B1D5-4C69-A45C-8DE151D92E0E}"/>
-    <hyperlink ref="N7" r:id="rId104" xr:uid="{9145B996-5C7D-41D0-98E1-0B9580548640}"/>
-    <hyperlink ref="N9" r:id="rId105" xr:uid="{86E8ED18-9ACB-4182-BE42-F0985D16B622}"/>
-    <hyperlink ref="N12" r:id="rId106" xr:uid="{8D7B7EA7-60FD-4946-A4ED-BF183B55C888}"/>
-    <hyperlink ref="N13" r:id="rId107" xr:uid="{BC286704-8307-4834-BEB6-C04D8FD0A586}"/>
-    <hyperlink ref="D10" r:id="rId108" xr:uid="{B2A72DB3-C272-420C-A469-E954856A6B08}"/>
-    <hyperlink ref="D11" r:id="rId109" xr:uid="{8BC3FEBB-B9AB-4D98-8EDF-7CD8DC779BF4}"/>
-    <hyperlink ref="E10" r:id="rId110" xr:uid="{6E28A39C-02BF-49C5-98D4-A9C4CFE9759B}"/>
-    <hyperlink ref="E11" r:id="rId111" xr:uid="{9A9F9B97-A5DA-4BA9-8388-996087A5F8B4}"/>
-    <hyperlink ref="F10" r:id="rId112" xr:uid="{BC5D07AE-CB2B-4A26-879F-2C0346CEDAC0}"/>
-    <hyperlink ref="F11" r:id="rId113" xr:uid="{19E0F53D-AF2F-4383-B069-3692FCABB95C}"/>
-    <hyperlink ref="G10" r:id="rId114" xr:uid="{8EB4D110-9450-40E1-9235-02E97342DC65}"/>
-    <hyperlink ref="G11" r:id="rId115" xr:uid="{E076B0D9-7B6F-4FCC-86B7-CFD566D4F0C3}"/>
-    <hyperlink ref="K4" r:id="rId116" xr:uid="{21264E62-7D55-4570-B7F3-14A8C1F94554}"/>
-    <hyperlink ref="K5" r:id="rId117" xr:uid="{27B8D1A0-3BEC-4886-8B21-278E4172F1AC}"/>
-    <hyperlink ref="K6" r:id="rId118" xr:uid="{4CF8DD02-3CED-43BD-847F-8D08F47CDAE1}"/>
-    <hyperlink ref="K7" r:id="rId119" xr:uid="{20C17813-8DDD-41E5-A174-604C4E03AE94}"/>
-    <hyperlink ref="K9" r:id="rId120" xr:uid="{B61181A8-4BEA-4F2D-85A4-C991B7B7A420}"/>
-    <hyperlink ref="K12" r:id="rId121" xr:uid="{03DFEAB3-E7DD-41B4-BFF8-7F95B3A377BA}"/>
-    <hyperlink ref="K13" r:id="rId122" xr:uid="{4F5B7C15-A4CB-4F2F-B65C-4465D06D5E10}"/>
-    <hyperlink ref="K15" r:id="rId123" xr:uid="{22C32313-A6BB-4638-A54C-7A989659D8E9}"/>
-    <hyperlink ref="K16" r:id="rId124" xr:uid="{B88BC585-4723-4F16-917D-CFB79E8E2808}"/>
-    <hyperlink ref="K1" r:id="rId125" display="https://community.infineon.com/t5/Cypress-Partner-Module-Support/Cypress-Linux-FMAC-Fafnir/ta-p/390153" xr:uid="{EF8836DE-086E-47CB-A007-2FE65D5A40CC}"/>
-    <hyperlink ref="T1" r:id="rId126" display="https://community.infineon.com/t5/Knowledge-Base-Articles/Cypress-Linux-WiFi-Driver-Release-FMAC-2018-07-16/ta-p/251360" xr:uid="{8D952104-5F6E-448D-89EC-6776F31A2A6C}"/>
-    <hyperlink ref="S1" r:id="rId127" display="https://community.infineon.com/t5/Knowledge-Base-Articles/Cypress-Linux-WiFi-Driver-Release-FMAC-2018-09-28/ta-p/253878" xr:uid="{411C4CB8-2E35-4803-A537-CCFE1E5BC664}"/>
-    <hyperlink ref="R1" r:id="rId128" display="https://community.infineon.com/t5/Knowledge-Base-Articles/Cypress-Linux-WiFi-Driver-Release-FMAC-2020-01-15/ta-p/248507" xr:uid="{5D1629B7-807D-4C9F-BB5E-DC2135882763}"/>
-    <hyperlink ref="Q1" r:id="rId129" display="https://community.infineon.com/t5/Knowledge-Base-Articles/Cypress-Linux-WiFi-Driver-Release-FMAC-2020-06-25/ta-p/252500" xr:uid="{CB693B9A-CCFA-4256-AFA0-B47F7C315C32}"/>
-    <hyperlink ref="P1" r:id="rId130" display="https://community.infineon.com/t5/Knowledge-Base-Articles/Cypress-Linux-WiFi-Driver-Release-FMAC-2020-09-25/ta-p/251089" xr:uid="{03991198-F7E4-4F0B-B83F-72E1444E38C2}"/>
-    <hyperlink ref="O1" r:id="rId131" display="https://github.com/Infineon/ifx-linux-wireless/tree/release-v5.4.18-2021_0527" xr:uid="{AF848772-4499-4096-BB2D-FDEF92537DFC}"/>
-    <hyperlink ref="N1" r:id="rId132" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.10.9-2021_1020" xr:uid="{C90BBEA6-0EF3-4C34-AFD2-C9A5733D2E38}"/>
-    <hyperlink ref="M1" r:id="rId133" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.10.9-2022_0511" xr:uid="{471F56C1-4A37-47D7-94D6-18AA97A8012E}"/>
-    <hyperlink ref="L1" r:id="rId134" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.10.9-2022_0909" xr:uid="{851E0494-BBF3-4C31-9D77-D496B6DC3F7A}"/>
-    <hyperlink ref="J1" r:id="rId135" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.15.58-2023_0222" xr:uid="{81EE05C5-19B1-4A43-8CFC-B38864650E32}"/>
-    <hyperlink ref="I1" r:id="rId136" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.15.58-2023_0523" xr:uid="{8527A864-F511-4E81-AE33-FDB76F25F2CF}"/>
-    <hyperlink ref="H1" r:id="rId137" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.15.58-2023_0801" xr:uid="{88E884E5-E7D0-4CFC-9109-FC29A5151621}"/>
-    <hyperlink ref="G1" r:id="rId138" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.15.58-2023_0901" xr:uid="{3C0719B5-D83B-4730-9A46-1BFBE26AC78A}"/>
-    <hyperlink ref="F1" r:id="rId139" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.15.58-2023_1128" xr:uid="{802E3126-91AD-490C-AA06-5E8639790410}"/>
-    <hyperlink ref="E1" r:id="rId140" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.15.58-2024_0514" xr:uid="{AE92591C-D1B7-4FA6-9B7D-8AB8CCAB1C00}"/>
-    <hyperlink ref="D1" r:id="rId141" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v6.1.97-2024_1115" xr:uid="{ED0AE27C-8EDF-4AB0-AA96-4165DD625542}"/>
-    <hyperlink ref="K2" r:id="rId142" xr:uid="{64D11300-1C82-4871-89AB-8562E0CBC5E4}"/>
-    <hyperlink ref="D4" r:id="rId143" xr:uid="{41E7F86F-674E-4FFC-B622-626E7E50281A}"/>
-    <hyperlink ref="E4" r:id="rId144" xr:uid="{6CACCABF-8DE8-4C5B-9FDC-FC41F5AA7173}"/>
-    <hyperlink ref="F4" r:id="rId145" xr:uid="{DA24608D-1F2F-430E-BA03-372CA8A37DD4}"/>
-    <hyperlink ref="G4" r:id="rId146" xr:uid="{25FD38A3-A738-421B-9C5C-3074805648B3}"/>
-    <hyperlink ref="H4" r:id="rId147" xr:uid="{7FA63980-29E8-45D5-9E6C-33885F64B6C1}"/>
-    <hyperlink ref="I4" r:id="rId148" xr:uid="{A47BD8E8-B80A-4717-A734-B4C9A1D3021A}"/>
-    <hyperlink ref="J4" r:id="rId149" xr:uid="{FE296B63-9DD7-4335-B029-3FFF3780ECF5}"/>
-    <hyperlink ref="E6:F6" r:id="rId150" display="7.45.265" xr:uid="{F55B93F8-B8F9-45E5-97CC-C73ECAB209E2}"/>
-    <hyperlink ref="H6:J6" r:id="rId151" display="7.45.251" xr:uid="{3EE3DAC8-8F3F-4434-AA90-0F2B10B260DA}"/>
-    <hyperlink ref="J10" r:id="rId152" xr:uid="{F247879E-700D-40F3-B83F-DE81BD9C9FE6}"/>
-    <hyperlink ref="J11" r:id="rId153" xr:uid="{FD44CA84-5222-4EBC-A01D-73449C6EBEE1}"/>
-    <hyperlink ref="L10" r:id="rId154" xr:uid="{57518D84-6F7D-4F5A-A4CC-446AA9A28E6B}"/>
-    <hyperlink ref="L11" r:id="rId155" xr:uid="{7C0572E5-B75E-4285-9A52-87761581D4A1}"/>
-    <hyperlink ref="M10" r:id="rId156" xr:uid="{1ED57864-546B-4ABB-9D92-124F7ED69BEB}"/>
-    <hyperlink ref="M11" r:id="rId157" xr:uid="{255F663A-CD3E-4420-A413-196CA856DD25}"/>
-    <hyperlink ref="N11" r:id="rId158" xr:uid="{EC643B11-D503-4F2F-BC28-3E9DD787EF33}"/>
-    <hyperlink ref="O2" r:id="rId159" xr:uid="{0D98EBC7-EB17-4E10-BD59-04C2B43014F7}"/>
-    <hyperlink ref="O4" r:id="rId160" xr:uid="{F2A25523-9665-4F41-9F63-81F578993A7B}"/>
-    <hyperlink ref="O6" r:id="rId161" xr:uid="{D2A74D62-4A82-421E-960B-6861E30612C5}"/>
-    <hyperlink ref="O7" r:id="rId162" xr:uid="{2F3D8DF7-B0D2-4F2A-95EF-AE840D6D8EC3}"/>
-    <hyperlink ref="O12" r:id="rId163" xr:uid="{5E7B9BBA-E1D6-475D-8AA7-06503F6F1671}"/>
-    <hyperlink ref="O13" r:id="rId164" xr:uid="{57A87C99-3278-4548-BF49-74F6B39DD225}"/>
+    <hyperlink ref="P2" r:id="rId1"/>
+    <hyperlink ref="P4" r:id="rId2"/>
+    <hyperlink ref="P6" r:id="rId3"/>
+    <hyperlink ref="P7" r:id="rId4"/>
+    <hyperlink ref="Q2" r:id="rId5"/>
+    <hyperlink ref="Q4" r:id="rId6"/>
+    <hyperlink ref="Q6" r:id="rId7"/>
+    <hyperlink ref="Q7" r:id="rId8"/>
+    <hyperlink ref="Q12" r:id="rId9"/>
+    <hyperlink ref="Q13" r:id="rId10"/>
+    <hyperlink ref="R2" r:id="rId11"/>
+    <hyperlink ref="R4" r:id="rId12"/>
+    <hyperlink ref="R6" r:id="rId13"/>
+    <hyperlink ref="R7" r:id="rId14"/>
+    <hyperlink ref="S2" r:id="rId15"/>
+    <hyperlink ref="S4" r:id="rId16"/>
+    <hyperlink ref="S6" r:id="rId17"/>
+    <hyperlink ref="T2" r:id="rId18"/>
+    <hyperlink ref="T4" r:id="rId19"/>
+    <hyperlink ref="T6" r:id="rId20"/>
+    <hyperlink ref="D2" r:id="rId21"/>
+    <hyperlink ref="D3" r:id="rId22"/>
+    <hyperlink ref="D5" r:id="rId23"/>
+    <hyperlink ref="D6" r:id="rId24"/>
+    <hyperlink ref="D7" r:id="rId25"/>
+    <hyperlink ref="D9" r:id="rId26"/>
+    <hyperlink ref="D12" r:id="rId27"/>
+    <hyperlink ref="D13" r:id="rId28"/>
+    <hyperlink ref="D15" r:id="rId29"/>
+    <hyperlink ref="D16" r:id="rId30"/>
+    <hyperlink ref="E2" r:id="rId31"/>
+    <hyperlink ref="E3" r:id="rId32"/>
+    <hyperlink ref="D14" r:id="rId33"/>
+    <hyperlink ref="E5" r:id="rId34"/>
+    <hyperlink ref="E7" r:id="rId35"/>
+    <hyperlink ref="E9" r:id="rId36"/>
+    <hyperlink ref="E12" r:id="rId37"/>
+    <hyperlink ref="E13" r:id="rId38"/>
+    <hyperlink ref="E15" r:id="rId39"/>
+    <hyperlink ref="E16" r:id="rId40"/>
+    <hyperlink ref="F2" r:id="rId41"/>
+    <hyperlink ref="F5" r:id="rId42"/>
+    <hyperlink ref="F7" r:id="rId43"/>
+    <hyperlink ref="F9" r:id="rId44"/>
+    <hyperlink ref="F12" r:id="rId45"/>
+    <hyperlink ref="F13" r:id="rId46" display="18.53.284.17"/>
+    <hyperlink ref="F15" r:id="rId47"/>
+    <hyperlink ref="F16" r:id="rId48"/>
+    <hyperlink ref="G2" r:id="rId49"/>
+    <hyperlink ref="G5" r:id="rId50"/>
+    <hyperlink ref="G6" r:id="rId51"/>
+    <hyperlink ref="G7" r:id="rId52"/>
+    <hyperlink ref="G9" r:id="rId53"/>
+    <hyperlink ref="G12" r:id="rId54"/>
+    <hyperlink ref="G13" r:id="rId55"/>
+    <hyperlink ref="G15" r:id="rId56"/>
+    <hyperlink ref="G16" r:id="rId57"/>
+    <hyperlink ref="H2" r:id="rId58"/>
+    <hyperlink ref="H5" r:id="rId59"/>
+    <hyperlink ref="H7" r:id="rId60"/>
+    <hyperlink ref="H9" r:id="rId61"/>
+    <hyperlink ref="H12" r:id="rId62"/>
+    <hyperlink ref="H13" r:id="rId63"/>
+    <hyperlink ref="H15" r:id="rId64"/>
+    <hyperlink ref="H16" r:id="rId65"/>
+    <hyperlink ref="I2" r:id="rId66"/>
+    <hyperlink ref="I5" r:id="rId67"/>
+    <hyperlink ref="I7" r:id="rId68"/>
+    <hyperlink ref="I9" r:id="rId69"/>
+    <hyperlink ref="I12" r:id="rId70"/>
+    <hyperlink ref="I13" r:id="rId71"/>
+    <hyperlink ref="I15" r:id="rId72"/>
+    <hyperlink ref="I16" r:id="rId73"/>
+    <hyperlink ref="J2" r:id="rId74"/>
+    <hyperlink ref="J5" r:id="rId75"/>
+    <hyperlink ref="J7" r:id="rId76"/>
+    <hyperlink ref="J9" r:id="rId77"/>
+    <hyperlink ref="J12" r:id="rId78"/>
+    <hyperlink ref="J13" r:id="rId79"/>
+    <hyperlink ref="J15" r:id="rId80"/>
+    <hyperlink ref="J16" r:id="rId81"/>
+    <hyperlink ref="L2" r:id="rId82"/>
+    <hyperlink ref="L4" r:id="rId83"/>
+    <hyperlink ref="L5" r:id="rId84"/>
+    <hyperlink ref="L6" r:id="rId85"/>
+    <hyperlink ref="L7" r:id="rId86"/>
+    <hyperlink ref="L9" r:id="rId87"/>
+    <hyperlink ref="L12" r:id="rId88"/>
+    <hyperlink ref="L13" r:id="rId89"/>
+    <hyperlink ref="L15" r:id="rId90"/>
+    <hyperlink ref="L16" r:id="rId91"/>
+    <hyperlink ref="M2" r:id="rId92"/>
+    <hyperlink ref="M4" r:id="rId93"/>
+    <hyperlink ref="M5" r:id="rId94"/>
+    <hyperlink ref="M6" r:id="rId95"/>
+    <hyperlink ref="M7" r:id="rId96"/>
+    <hyperlink ref="M9" r:id="rId97"/>
+    <hyperlink ref="M12" r:id="rId98"/>
+    <hyperlink ref="M13" r:id="rId99"/>
+    <hyperlink ref="N2" r:id="rId100"/>
+    <hyperlink ref="N4" r:id="rId101"/>
+    <hyperlink ref="N5" r:id="rId102"/>
+    <hyperlink ref="N6" r:id="rId103"/>
+    <hyperlink ref="N7" r:id="rId104"/>
+    <hyperlink ref="N9" r:id="rId105"/>
+    <hyperlink ref="N12" r:id="rId106"/>
+    <hyperlink ref="N13" r:id="rId107"/>
+    <hyperlink ref="D10" r:id="rId108"/>
+    <hyperlink ref="D11" r:id="rId109"/>
+    <hyperlink ref="E10" r:id="rId110"/>
+    <hyperlink ref="E11" r:id="rId111"/>
+    <hyperlink ref="F10" r:id="rId112"/>
+    <hyperlink ref="F11" r:id="rId113"/>
+    <hyperlink ref="G10" r:id="rId114"/>
+    <hyperlink ref="G11" r:id="rId115"/>
+    <hyperlink ref="K4" r:id="rId116"/>
+    <hyperlink ref="K5" r:id="rId117"/>
+    <hyperlink ref="K6" r:id="rId118"/>
+    <hyperlink ref="K7" r:id="rId119"/>
+    <hyperlink ref="K9" r:id="rId120"/>
+    <hyperlink ref="K12" r:id="rId121"/>
+    <hyperlink ref="K13" r:id="rId122"/>
+    <hyperlink ref="K15" r:id="rId123"/>
+    <hyperlink ref="K16" r:id="rId124"/>
+    <hyperlink ref="K1" r:id="rId125" display="https://community.infineon.com/t5/Cypress-Partner-Module-Support/Cypress-Linux-FMAC-Fafnir/ta-p/390153"/>
+    <hyperlink ref="T1" r:id="rId126" display="https://community.infineon.com/t5/Knowledge-Base-Articles/Cypress-Linux-WiFi-Driver-Release-FMAC-2018-07-16/ta-p/251360"/>
+    <hyperlink ref="S1" r:id="rId127" display="https://community.infineon.com/t5/Knowledge-Base-Articles/Cypress-Linux-WiFi-Driver-Release-FMAC-2018-09-28/ta-p/253878"/>
+    <hyperlink ref="R1" r:id="rId128" display="https://community.infineon.com/t5/Knowledge-Base-Articles/Cypress-Linux-WiFi-Driver-Release-FMAC-2020-01-15/ta-p/248507"/>
+    <hyperlink ref="Q1" r:id="rId129" display="https://community.infineon.com/t5/Knowledge-Base-Articles/Cypress-Linux-WiFi-Driver-Release-FMAC-2020-06-25/ta-p/252500"/>
+    <hyperlink ref="P1" r:id="rId130" display="https://community.infineon.com/t5/Knowledge-Base-Articles/Cypress-Linux-WiFi-Driver-Release-FMAC-2020-09-25/ta-p/251089"/>
+    <hyperlink ref="O1" r:id="rId131" display="https://github.com/Infineon/ifx-linux-wireless/tree/release-v5.4.18-2021_0527"/>
+    <hyperlink ref="N1" r:id="rId132" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.10.9-2021_1020"/>
+    <hyperlink ref="M1" r:id="rId133" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.10.9-2022_0511"/>
+    <hyperlink ref="L1" r:id="rId134" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.10.9-2022_0909"/>
+    <hyperlink ref="J1" r:id="rId135" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.15.58-2023_0222"/>
+    <hyperlink ref="I1" r:id="rId136" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.15.58-2023_0523"/>
+    <hyperlink ref="H1" r:id="rId137" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.15.58-2023_0801"/>
+    <hyperlink ref="G1" r:id="rId138" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.15.58-2023_0901"/>
+    <hyperlink ref="F1" r:id="rId139" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.15.58-2023_1128"/>
+    <hyperlink ref="E1" r:id="rId140" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.15.58-2024_0514"/>
+    <hyperlink ref="D1" r:id="rId141" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v6.1.97-2024_1115"/>
+    <hyperlink ref="K2" r:id="rId142"/>
+    <hyperlink ref="D4" r:id="rId143"/>
+    <hyperlink ref="E4" r:id="rId144"/>
+    <hyperlink ref="F4" r:id="rId145"/>
+    <hyperlink ref="G4" r:id="rId146"/>
+    <hyperlink ref="H4" r:id="rId147"/>
+    <hyperlink ref="I4" r:id="rId148"/>
+    <hyperlink ref="J4" r:id="rId149"/>
+    <hyperlink ref="E6:F6" r:id="rId150" display="7.45.265"/>
+    <hyperlink ref="H6:J6" r:id="rId151" display="7.45.251"/>
+    <hyperlink ref="J10" r:id="rId152"/>
+    <hyperlink ref="J11" r:id="rId153"/>
+    <hyperlink ref="L10" r:id="rId154"/>
+    <hyperlink ref="L11" r:id="rId155"/>
+    <hyperlink ref="M10" r:id="rId156"/>
+    <hyperlink ref="M11" r:id="rId157"/>
+    <hyperlink ref="N11" r:id="rId158"/>
+    <hyperlink ref="O2" r:id="rId159"/>
+    <hyperlink ref="O4" r:id="rId160"/>
+    <hyperlink ref="O6" r:id="rId161"/>
+    <hyperlink ref="O7" r:id="rId162"/>
+    <hyperlink ref="O12" r:id="rId163"/>
+    <hyperlink ref="O13" r:id="rId164"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId165"/>
@@ -3003,12 +3001,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e6dc366e-c0b9-431d-9cd1-ef5fdc68f744">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="0606b7e6-2769-4854-ad6a-0bb7c1ff72e3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3243,20 +3243,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e6dc366e-c0b9-431d-9cd1-ef5fdc68f744">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="0606b7e6-2769-4854-ad6a-0bb7c1ff72e3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E739B31-040A-4763-A34B-28A2ACB33BEF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E05F8D0-189F-4ADB-8361-F480A6B5BD0F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="230bf304-d62f-4465-a926-5dd49d1204ea"/>
+    <ds:schemaRef ds:uri="e6dc366e-c0b9-431d-9cd1-ef5fdc68f744"/>
+    <ds:schemaRef ds:uri="0606b7e6-2769-4854-ad6a-0bb7c1ff72e3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3281,13 +3283,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E05F8D0-189F-4ADB-8361-F480A6B5BD0F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E739B31-040A-4763-A34B-28A2ACB33BEF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="230bf304-d62f-4465-a926-5dd49d1204ea"/>
-    <ds:schemaRef ds:uri="e6dc366e-c0b9-431d-9cd1-ef5fdc68f744"/>
-    <ds:schemaRef ds:uri="0606b7e6-2769-4854-ad6a-0bb7c1ff72e3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated FW location information
</commit_message>
<xml_diff>
--- a/FMAC_FW_Versions.xlsx
+++ b/FMAC_FW_Versions.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MEAASC01\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Projects\Murata\In progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B522FA8A-6BD5-407B-BE0D-65B137748B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28860" windowHeight="11220"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,28 +20,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Romit Chatterjee</author>
   </authors>
   <commentList>
-    <comment ref="G2" authorId="0" shapeId="0">
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -69,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="135">
   <si>
     <t>13.10.271.138</t>
   </si>
@@ -475,25 +465,28 @@
     <t>2BZ</t>
   </si>
   <si>
-    <t>(2) For 2AE-USB, rename the "cyfmac4373-usb.2AE.bin" FW file to "cyfmac4373-usb.bin" before using.</t>
-  </si>
-  <si>
-    <t>(3) For 2BC-USB, rename the "cyfmac4373-usb.2BC.bin" FW file to "cyfmac4373-usb.bin" before using.</t>
-  </si>
-  <si>
-    <t>(4) For Godzilla (3) release, the FW versions for 1LV, 2AE and 2BC were changed incorrectly. These were corrected in the next release (Hedorah).</t>
-  </si>
-  <si>
     <t>1XA/2BA</t>
   </si>
   <si>
-    <t>(5) If you are using Godzilla, it is recommened to use the latest iteration of the driver (Godzilla 3). Same for Fafnir (Fafnir 2)</t>
+    <t>(2) For 2AE-USB, rename the "cyfmac4373-usb.2AE.bin" FW file to "cyfmac4373.bin" before using.</t>
+  </si>
+  <si>
+    <t>(3) For 2BC-USB, rename the "cyfmac4373-usb.2BC.bin" FW file to "cyfmac4373.bin" before using.</t>
+  </si>
+  <si>
+    <t>(4) Same firmware file (cyfmac54591-sdio.bin) is used for 2BZ and 1XA. 2BZ is based out of IFX chipset 54590.</t>
+  </si>
+  <si>
+    <t>(5) For Godzilla (3) release, the FW versions for 1LV, 2AE and 2BC were changed incorrectly. These were corrected in the next release (Hedorah).</t>
+  </si>
+  <si>
+    <t>(6) If you are using Godzilla, it is recommened to use the latest iteration of the driver (Godzilla 3). Same for Fafnir (Fafnir 2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1290,7 +1283,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Table Style 1" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Table Style 1" pivot="0" count="1">
+    <tableStyle name="Table Style 1" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="headerRow" dxfId="24"/>
     </tableStyle>
   </tableStyles>
@@ -1312,32 +1305,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:T16" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
-  <autoFilter ref="A1:T16"/>
-  <sortState ref="A2:T16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:T16" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+  <autoFilter ref="A1:T16" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T16">
     <sortCondition ref="A1:A16"/>
   </sortState>
   <tableColumns count="20">
-    <tableColumn id="1" name="FW name" dataDxfId="19"/>
-    <tableColumn id="2" name="Module" dataDxfId="18"/>
-    <tableColumn id="3" name="Chipset" dataDxfId="17"/>
-    <tableColumn id="20" name="Jaculus_x000a_(v6.1.97-2024_1115)" dataDxfId="16" dataCellStyle="Hyperlink"/>
-    <tableColumn id="19" name="Indrik_x000a_(v5.15.58-2024_0514)" dataDxfId="15" dataCellStyle="Hyperlink"/>
-    <tableColumn id="18" name="Hedorah_x000a_(v5.15.58-2023_1128)" dataDxfId="14" dataCellStyle="Hyperlink"/>
-    <tableColumn id="17" name="Godzilla 3_x000a_(v5.15.58-2023_0901)" dataDxfId="13" dataCellStyle="Hyperlink"/>
-    <tableColumn id="16" name="Godzilla 2_x000a_(v5.15.58-2023_0801)" dataDxfId="12" dataCellStyle="Hyperlink"/>
-    <tableColumn id="15" name="Godzilla_x000a_(v5.15.58-2023_0523)" dataDxfId="11" dataCellStyle="Hyperlink"/>
-    <tableColumn id="14" name="Fafnir 2_x000a_(v5.15.58-2023_0222)" dataDxfId="10" dataCellStyle="Hyperlink"/>
-    <tableColumn id="13" name="Fafnir_x000a_(v5.15.58-20221223)" dataDxfId="9" dataCellStyle="Hyperlink"/>
-    <tableColumn id="12" name="Ebirah_x000a_(v5.10.9-2022_0909)" dataDxfId="8" dataCellStyle="Hyperlink"/>
-    <tableColumn id="11" name="Drogon_x000a_(v5.10.9-2022_0511)" dataDxfId="7" dataCellStyle="Hyperlink"/>
-    <tableColumn id="10" name="Cynder_x000a_(v5.10.9-2021_1020)" dataDxfId="6"/>
-    <tableColumn id="9" name="Baragon_x000a_(v5.4.18-2021_0527)" dataDxfId="5"/>
-    <tableColumn id="8" name="Spiga_x000a_(v5.4.18-2020_0925)" dataDxfId="4"/>
-    <tableColumn id="7" name="Zigra_x000a_(v5.4.18-2020_0625)" dataDxfId="3"/>
-    <tableColumn id="6" name="Kong_x000a_(v4.14.77-2020_0115)" dataDxfId="2"/>
-    <tableColumn id="5" name="Manda_x000a_(v4.14.52-2018_0928)" dataDxfId="1"/>
-    <tableColumn id="4" name="Mothra_x000a_(v4.14.34-2018_0716)" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="FW name" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Module" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Chipset" dataDxfId="17"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Jaculus_x000a_(v6.1.97-2024_1115)" dataDxfId="16" dataCellStyle="Hyperlink"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Indrik_x000a_(v5.15.58-2024_0514)" dataDxfId="15" dataCellStyle="Hyperlink"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Hedorah_x000a_(v5.15.58-2023_1128)" dataDxfId="14" dataCellStyle="Hyperlink"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Godzilla 3_x000a_(v5.15.58-2023_0901)" dataDxfId="13" dataCellStyle="Hyperlink"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Godzilla 2_x000a_(v5.15.58-2023_0801)" dataDxfId="12" dataCellStyle="Hyperlink"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Godzilla_x000a_(v5.15.58-2023_0523)" dataDxfId="11" dataCellStyle="Hyperlink"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Fafnir 2_x000a_(v5.15.58-2023_0222)" dataDxfId="10" dataCellStyle="Hyperlink"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Fafnir_x000a_(v5.15.58-20221223)" dataDxfId="9" dataCellStyle="Hyperlink"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Ebirah_x000a_(v5.10.9-2022_0909)" dataDxfId="8" dataCellStyle="Hyperlink"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Drogon_x000a_(v5.10.9-2022_0511)" dataDxfId="7" dataCellStyle="Hyperlink"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Cynder_x000a_(v5.10.9-2021_1020)" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Baragon_x000a_(v5.4.18-2021_0527)" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Spiga_x000a_(v5.4.18-2020_0925)" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Zigra_x000a_(v5.4.18-2020_0625)" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Kong_x000a_(v4.14.77-2020_0115)" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Manda_x000a_(v4.14.52-2018_0928)" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Mothra_x000a_(v4.14.34-2018_0716)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1639,14 +1632,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:MQ23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:MQ24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2568,7 +2561,7 @@
         <v>85</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C12" s="4">
         <v>54591</v>
@@ -2805,17 +2798,17 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
@@ -2823,173 +2816,178 @@
         <v>133</v>
       </c>
     </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>134</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1"/>
-    <hyperlink ref="P4" r:id="rId2"/>
-    <hyperlink ref="P6" r:id="rId3"/>
-    <hyperlink ref="P7" r:id="rId4"/>
-    <hyperlink ref="Q2" r:id="rId5"/>
-    <hyperlink ref="Q4" r:id="rId6"/>
-    <hyperlink ref="Q6" r:id="rId7"/>
-    <hyperlink ref="Q7" r:id="rId8"/>
-    <hyperlink ref="Q12" r:id="rId9"/>
-    <hyperlink ref="Q13" r:id="rId10"/>
-    <hyperlink ref="R2" r:id="rId11"/>
-    <hyperlink ref="R4" r:id="rId12"/>
-    <hyperlink ref="R6" r:id="rId13"/>
-    <hyperlink ref="R7" r:id="rId14"/>
-    <hyperlink ref="S2" r:id="rId15"/>
-    <hyperlink ref="S4" r:id="rId16"/>
-    <hyperlink ref="S6" r:id="rId17"/>
-    <hyperlink ref="T2" r:id="rId18"/>
-    <hyperlink ref="T4" r:id="rId19"/>
-    <hyperlink ref="T6" r:id="rId20"/>
-    <hyperlink ref="D2" r:id="rId21"/>
-    <hyperlink ref="D3" r:id="rId22"/>
-    <hyperlink ref="D5" r:id="rId23"/>
-    <hyperlink ref="D6" r:id="rId24"/>
-    <hyperlink ref="D7" r:id="rId25"/>
-    <hyperlink ref="D9" r:id="rId26"/>
-    <hyperlink ref="D12" r:id="rId27"/>
-    <hyperlink ref="D13" r:id="rId28"/>
-    <hyperlink ref="D15" r:id="rId29"/>
-    <hyperlink ref="D16" r:id="rId30"/>
-    <hyperlink ref="E2" r:id="rId31"/>
-    <hyperlink ref="E3" r:id="rId32"/>
-    <hyperlink ref="D14" r:id="rId33"/>
-    <hyperlink ref="E5" r:id="rId34"/>
-    <hyperlink ref="E7" r:id="rId35"/>
-    <hyperlink ref="E9" r:id="rId36"/>
-    <hyperlink ref="E12" r:id="rId37"/>
-    <hyperlink ref="E13" r:id="rId38"/>
-    <hyperlink ref="E15" r:id="rId39"/>
-    <hyperlink ref="E16" r:id="rId40"/>
-    <hyperlink ref="F2" r:id="rId41"/>
-    <hyperlink ref="F5" r:id="rId42"/>
-    <hyperlink ref="F7" r:id="rId43"/>
-    <hyperlink ref="F9" r:id="rId44"/>
-    <hyperlink ref="F12" r:id="rId45"/>
-    <hyperlink ref="F13" r:id="rId46" display="18.53.284.17"/>
-    <hyperlink ref="F15" r:id="rId47"/>
-    <hyperlink ref="F16" r:id="rId48"/>
-    <hyperlink ref="G2" r:id="rId49"/>
-    <hyperlink ref="G5" r:id="rId50"/>
-    <hyperlink ref="G6" r:id="rId51"/>
-    <hyperlink ref="G7" r:id="rId52"/>
-    <hyperlink ref="G9" r:id="rId53"/>
-    <hyperlink ref="G12" r:id="rId54"/>
-    <hyperlink ref="G13" r:id="rId55"/>
-    <hyperlink ref="G15" r:id="rId56"/>
-    <hyperlink ref="G16" r:id="rId57"/>
-    <hyperlink ref="H2" r:id="rId58"/>
-    <hyperlink ref="H5" r:id="rId59"/>
-    <hyperlink ref="H7" r:id="rId60"/>
-    <hyperlink ref="H9" r:id="rId61"/>
-    <hyperlink ref="H12" r:id="rId62"/>
-    <hyperlink ref="H13" r:id="rId63"/>
-    <hyperlink ref="H15" r:id="rId64"/>
-    <hyperlink ref="H16" r:id="rId65"/>
-    <hyperlink ref="I2" r:id="rId66"/>
-    <hyperlink ref="I5" r:id="rId67"/>
-    <hyperlink ref="I7" r:id="rId68"/>
-    <hyperlink ref="I9" r:id="rId69"/>
-    <hyperlink ref="I12" r:id="rId70"/>
-    <hyperlink ref="I13" r:id="rId71"/>
-    <hyperlink ref="I15" r:id="rId72"/>
-    <hyperlink ref="I16" r:id="rId73"/>
-    <hyperlink ref="J2" r:id="rId74"/>
-    <hyperlink ref="J5" r:id="rId75"/>
-    <hyperlink ref="J7" r:id="rId76"/>
-    <hyperlink ref="J9" r:id="rId77"/>
-    <hyperlink ref="J12" r:id="rId78"/>
-    <hyperlink ref="J13" r:id="rId79"/>
-    <hyperlink ref="J15" r:id="rId80"/>
-    <hyperlink ref="J16" r:id="rId81"/>
-    <hyperlink ref="L2" r:id="rId82"/>
-    <hyperlink ref="L4" r:id="rId83"/>
-    <hyperlink ref="L5" r:id="rId84"/>
-    <hyperlink ref="L6" r:id="rId85"/>
-    <hyperlink ref="L7" r:id="rId86"/>
-    <hyperlink ref="L9" r:id="rId87"/>
-    <hyperlink ref="L12" r:id="rId88"/>
-    <hyperlink ref="L13" r:id="rId89"/>
-    <hyperlink ref="L15" r:id="rId90"/>
-    <hyperlink ref="L16" r:id="rId91"/>
-    <hyperlink ref="M2" r:id="rId92"/>
-    <hyperlink ref="M4" r:id="rId93"/>
-    <hyperlink ref="M5" r:id="rId94"/>
-    <hyperlink ref="M6" r:id="rId95"/>
-    <hyperlink ref="M7" r:id="rId96"/>
-    <hyperlink ref="M9" r:id="rId97"/>
-    <hyperlink ref="M12" r:id="rId98"/>
-    <hyperlink ref="M13" r:id="rId99"/>
-    <hyperlink ref="N2" r:id="rId100"/>
-    <hyperlink ref="N4" r:id="rId101"/>
-    <hyperlink ref="N5" r:id="rId102"/>
-    <hyperlink ref="N6" r:id="rId103"/>
-    <hyperlink ref="N7" r:id="rId104"/>
-    <hyperlink ref="N9" r:id="rId105"/>
-    <hyperlink ref="N12" r:id="rId106"/>
-    <hyperlink ref="N13" r:id="rId107"/>
-    <hyperlink ref="D10" r:id="rId108"/>
-    <hyperlink ref="D11" r:id="rId109"/>
-    <hyperlink ref="E10" r:id="rId110"/>
-    <hyperlink ref="E11" r:id="rId111"/>
-    <hyperlink ref="F10" r:id="rId112"/>
-    <hyperlink ref="F11" r:id="rId113"/>
-    <hyperlink ref="G10" r:id="rId114"/>
-    <hyperlink ref="G11" r:id="rId115"/>
-    <hyperlink ref="K4" r:id="rId116"/>
-    <hyperlink ref="K5" r:id="rId117"/>
-    <hyperlink ref="K6" r:id="rId118"/>
-    <hyperlink ref="K7" r:id="rId119"/>
-    <hyperlink ref="K9" r:id="rId120"/>
-    <hyperlink ref="K12" r:id="rId121"/>
-    <hyperlink ref="K13" r:id="rId122"/>
-    <hyperlink ref="K15" r:id="rId123"/>
-    <hyperlink ref="K16" r:id="rId124"/>
-    <hyperlink ref="K1" r:id="rId125" display="https://community.infineon.com/t5/Cypress-Partner-Module-Support/Cypress-Linux-FMAC-Fafnir/ta-p/390153"/>
-    <hyperlink ref="T1" r:id="rId126" display="https://community.infineon.com/t5/Knowledge-Base-Articles/Cypress-Linux-WiFi-Driver-Release-FMAC-2018-07-16/ta-p/251360"/>
-    <hyperlink ref="S1" r:id="rId127" display="https://community.infineon.com/t5/Knowledge-Base-Articles/Cypress-Linux-WiFi-Driver-Release-FMAC-2018-09-28/ta-p/253878"/>
-    <hyperlink ref="R1" r:id="rId128" display="https://community.infineon.com/t5/Knowledge-Base-Articles/Cypress-Linux-WiFi-Driver-Release-FMAC-2020-01-15/ta-p/248507"/>
-    <hyperlink ref="Q1" r:id="rId129" display="https://community.infineon.com/t5/Knowledge-Base-Articles/Cypress-Linux-WiFi-Driver-Release-FMAC-2020-06-25/ta-p/252500"/>
-    <hyperlink ref="P1" r:id="rId130" display="https://community.infineon.com/t5/Knowledge-Base-Articles/Cypress-Linux-WiFi-Driver-Release-FMAC-2020-09-25/ta-p/251089"/>
-    <hyperlink ref="O1" r:id="rId131" display="https://github.com/Infineon/ifx-linux-wireless/tree/release-v5.4.18-2021_0527"/>
-    <hyperlink ref="N1" r:id="rId132" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.10.9-2021_1020"/>
-    <hyperlink ref="M1" r:id="rId133" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.10.9-2022_0511"/>
-    <hyperlink ref="L1" r:id="rId134" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.10.9-2022_0909"/>
-    <hyperlink ref="J1" r:id="rId135" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.15.58-2023_0222"/>
-    <hyperlink ref="I1" r:id="rId136" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.15.58-2023_0523"/>
-    <hyperlink ref="H1" r:id="rId137" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.15.58-2023_0801"/>
-    <hyperlink ref="G1" r:id="rId138" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.15.58-2023_0901"/>
-    <hyperlink ref="F1" r:id="rId139" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.15.58-2023_1128"/>
-    <hyperlink ref="E1" r:id="rId140" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.15.58-2024_0514"/>
-    <hyperlink ref="D1" r:id="rId141" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v6.1.97-2024_1115"/>
-    <hyperlink ref="K2" r:id="rId142"/>
-    <hyperlink ref="D4" r:id="rId143"/>
-    <hyperlink ref="E4" r:id="rId144"/>
-    <hyperlink ref="F4" r:id="rId145"/>
-    <hyperlink ref="G4" r:id="rId146"/>
-    <hyperlink ref="H4" r:id="rId147"/>
-    <hyperlink ref="I4" r:id="rId148"/>
-    <hyperlink ref="J4" r:id="rId149"/>
-    <hyperlink ref="E6:F6" r:id="rId150" display="7.45.265"/>
-    <hyperlink ref="H6:J6" r:id="rId151" display="7.45.251"/>
-    <hyperlink ref="J10" r:id="rId152"/>
-    <hyperlink ref="J11" r:id="rId153"/>
-    <hyperlink ref="L10" r:id="rId154"/>
-    <hyperlink ref="L11" r:id="rId155"/>
-    <hyperlink ref="M10" r:id="rId156"/>
-    <hyperlink ref="M11" r:id="rId157"/>
-    <hyperlink ref="N11" r:id="rId158"/>
-    <hyperlink ref="O2" r:id="rId159"/>
-    <hyperlink ref="O4" r:id="rId160"/>
-    <hyperlink ref="O6" r:id="rId161"/>
-    <hyperlink ref="O7" r:id="rId162"/>
-    <hyperlink ref="O12" r:id="rId163"/>
-    <hyperlink ref="O13" r:id="rId164"/>
+    <hyperlink ref="P2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="P4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="P6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="P7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="Q2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="Q4" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="Q6" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="Q7" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="Q12" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="Q13" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="R2" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="R4" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="R6" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="R7" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="S2" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="S4" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="S6" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="T2" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="T4" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="T6" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="D2" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="D3" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="D5" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="D6" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="D7" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="D9" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="D12" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="D13" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="D15" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="D16" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="E2" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="E3" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="D14" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="E5" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="E7" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="E9" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="E12" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="E13" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="E15" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="E16" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="F2" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="F5" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="F7" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="F9" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="F12" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="F13" r:id="rId46" display="18.53.284.17" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="F15" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="F16" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="G2" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="G5" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="G6" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="G7" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="G9" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="G12" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="G13" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="G15" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="G16" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="H2" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="H5" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="H7" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="H9" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="H12" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="H13" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="H15" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="H16" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="I2" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="I5" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="I7" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="I9" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="I12" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="I13" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="I15" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="I16" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="J2" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="J5" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="J7" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="J9" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="J12" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="J13" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="J15" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="J16" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="L2" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="L4" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="L5" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="L6" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="L7" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="L9" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="L12" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="L13" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="L15" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="L16" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="M2" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="M4" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="M5" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="M6" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="M7" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="M9" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="M12" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="M13" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="N2" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="N4" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="N5" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="N6" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="N7" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="N9" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="N12" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="N13" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="D10" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="D11" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="E10" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="E11" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="F10" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="F11" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="G10" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="G11" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="K4" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="K5" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="K6" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="K7" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="K9" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="K12" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="K13" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="K15" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="K16" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="K1" r:id="rId125" display="https://community.infineon.com/t5/Cypress-Partner-Module-Support/Cypress-Linux-FMAC-Fafnir/ta-p/390153" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="T1" r:id="rId126" display="https://community.infineon.com/t5/Knowledge-Base-Articles/Cypress-Linux-WiFi-Driver-Release-FMAC-2018-07-16/ta-p/251360" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="S1" r:id="rId127" display="https://community.infineon.com/t5/Knowledge-Base-Articles/Cypress-Linux-WiFi-Driver-Release-FMAC-2018-09-28/ta-p/253878" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="R1" r:id="rId128" display="https://community.infineon.com/t5/Knowledge-Base-Articles/Cypress-Linux-WiFi-Driver-Release-FMAC-2020-01-15/ta-p/248507" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="Q1" r:id="rId129" display="https://community.infineon.com/t5/Knowledge-Base-Articles/Cypress-Linux-WiFi-Driver-Release-FMAC-2020-06-25/ta-p/252500" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="P1" r:id="rId130" display="https://community.infineon.com/t5/Knowledge-Base-Articles/Cypress-Linux-WiFi-Driver-Release-FMAC-2020-09-25/ta-p/251089" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="O1" r:id="rId131" display="https://github.com/Infineon/ifx-linux-wireless/tree/release-v5.4.18-2021_0527" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="N1" r:id="rId132" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.10.9-2021_1020" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="M1" r:id="rId133" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.10.9-2022_0511" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="L1" r:id="rId134" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.10.9-2022_0909" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="J1" r:id="rId135" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.15.58-2023_0222" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="I1" r:id="rId136" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.15.58-2023_0523" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="H1" r:id="rId137" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.15.58-2023_0801" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
+    <hyperlink ref="G1" r:id="rId138" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.15.58-2023_0901" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="F1" r:id="rId139" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.15.58-2023_1128" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="E1" r:id="rId140" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v5.15.58-2024_0514" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="D1" r:id="rId141" display="https://github.com/Infineon/ifx-wireless-drivers/tree/release-v6.1.97-2024_1115" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="K2" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="D4" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
+    <hyperlink ref="E4" r:id="rId144" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="F4" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
+    <hyperlink ref="G4" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="H4" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="I4" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="J4" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="E6:F6" r:id="rId150" display="7.45.265" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="H6:J6" r:id="rId151" display="7.45.251" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="J10" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="J11" r:id="rId153" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
+    <hyperlink ref="L10" r:id="rId154" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
+    <hyperlink ref="L11" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
+    <hyperlink ref="M10" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
+    <hyperlink ref="M11" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
+    <hyperlink ref="N11" r:id="rId158" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
+    <hyperlink ref="O2" r:id="rId159" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
+    <hyperlink ref="O4" r:id="rId160" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
+    <hyperlink ref="O6" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
+    <hyperlink ref="O7" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
+    <hyperlink ref="O12" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
+    <hyperlink ref="O13" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId165"/>
@@ -3001,14 +2999,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e6dc366e-c0b9-431d-9cd1-ef5fdc68f744">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="0606b7e6-2769-4854-ad6a-0bb7c1ff72e3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3243,22 +3239,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e6dc366e-c0b9-431d-9cd1-ef5fdc68f744">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="0606b7e6-2769-4854-ad6a-0bb7c1ff72e3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E05F8D0-189F-4ADB-8361-F480A6B5BD0F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E739B31-040A-4763-A34B-28A2ACB33BEF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="230bf304-d62f-4465-a926-5dd49d1204ea"/>
-    <ds:schemaRef ds:uri="e6dc366e-c0b9-431d-9cd1-ef5fdc68f744"/>
-    <ds:schemaRef ds:uri="0606b7e6-2769-4854-ad6a-0bb7c1ff72e3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3283,9 +3277,13 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E739B31-040A-4763-A34B-28A2ACB33BEF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E05F8D0-189F-4ADB-8361-F480A6B5BD0F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="230bf304-d62f-4465-a926-5dd49d1204ea"/>
+    <ds:schemaRef ds:uri="e6dc366e-c0b9-431d-9cd1-ef5fdc68f744"/>
+    <ds:schemaRef ds:uri="0606b7e6-2769-4854-ad6a-0bb7c1ff72e3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated 2FY Jaculus FW version
</commit_message>
<xml_diff>
--- a/FMAC_FW_Versions.xlsx
+++ b/FMAC_FW_Versions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Projects\Murata\In progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B522FA8A-6BD5-407B-BE0D-65B137748B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D56A56D-D6DB-48BE-9144-9FB8A8CA320E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -453,9 +453,6 @@
     <t>2FY</t>
   </si>
   <si>
-    <t>28.10.387.10</t>
-  </si>
-  <si>
     <t>7.95.48</t>
   </si>
   <si>
@@ -481,6 +478,9 @@
   </si>
   <si>
     <t>(6) If you are using Godzilla, it is recommened to use the latest iteration of the driver (Godzilla 3). Same for Fafnir (Fafnir 2)</t>
+  </si>
+  <si>
+    <t>28.10.387.16</t>
   </si>
 </sst>
 </file>
@@ -1639,7 +1639,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2153,7 +2153,7 @@
         <v>80</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C4" s="4">
         <v>43430</v>
@@ -2248,10 +2248,10 @@
         <v>91</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -2561,7 +2561,7 @@
         <v>85</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C12" s="4">
         <v>54591</v>
@@ -2615,7 +2615,7 @@
         <v>86</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C13" s="4">
         <v>54590</v>
@@ -2675,7 +2675,7 @@
         <v>55513</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -2798,27 +2798,27 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2999,12 +2999,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e6dc366e-c0b9-431d-9cd1-ef5fdc68f744">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="0606b7e6-2769-4854-ad6a-0bb7c1ff72e3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3239,20 +3241,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e6dc366e-c0b9-431d-9cd1-ef5fdc68f744">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="0606b7e6-2769-4854-ad6a-0bb7c1ff72e3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E739B31-040A-4763-A34B-28A2ACB33BEF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E05F8D0-189F-4ADB-8361-F480A6B5BD0F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="230bf304-d62f-4465-a926-5dd49d1204ea"/>
+    <ds:schemaRef ds:uri="e6dc366e-c0b9-431d-9cd1-ef5fdc68f744"/>
+    <ds:schemaRef ds:uri="0606b7e6-2769-4854-ad6a-0bb7c1ff72e3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3277,13 +3281,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E05F8D0-189F-4ADB-8361-F480A6B5BD0F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E739B31-040A-4763-A34B-28A2ACB33BEF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="230bf304-d62f-4465-a926-5dd49d1204ea"/>
-    <ds:schemaRef ds:uri="e6dc366e-c0b9-431d-9cd1-ef5fdc68f744"/>
-    <ds:schemaRef ds:uri="0606b7e6-2769-4854-ad6a-0bb7c1ff72e3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>